<commit_message>
Completed Set 9 and 10 sheets
</commit_message>
<xml_diff>
--- a/HCM_Core-Configurations.xlsx
+++ b/HCM_Core-Configurations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="15150" windowHeight="5325" tabRatio="603" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="15150" windowHeight="5325" tabRatio="603" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Configurations" sheetId="12" r:id="rId1"/>
@@ -17,12 +17,16 @@
     <sheet name="Manage Instance Qualifiers" sheetId="67" r:id="rId3"/>
     <sheet name="Manage Calendar Events" sheetId="69" r:id="rId4"/>
     <sheet name="Manage Profile Content Items" sheetId="68" r:id="rId5"/>
-    <sheet name="Manage Profile Rating Models" sheetId="70" r:id="rId6"/>
-    <sheet name="Manage Talent Notifications" sheetId="71" r:id="rId7"/>
-    <sheet name="Manage Work Shifts" sheetId="72" r:id="rId8"/>
+    <sheet name="Manage Position Trees" sheetId="73" r:id="rId6"/>
+    <sheet name="Manage Profile Types" sheetId="74" r:id="rId7"/>
+    <sheet name="Manage Profile Content Types" sheetId="75" r:id="rId8"/>
+    <sheet name="Manage EducationalEstab" sheetId="76" r:id="rId9"/>
+    <sheet name="Manage Profile Rating Models" sheetId="70" r:id="rId10"/>
+    <sheet name="Manage Talent Notifications" sheetId="71" r:id="rId11"/>
+    <sheet name="Manage Work Shifts" sheetId="72" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="Location">'[1]Optional Lists'!$F$9:$F$1815</definedName>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="412">
   <si>
     <t>Description</t>
   </si>
@@ -1051,17 +1055,238 @@
   </si>
   <si>
     <t>TI_ Performance Rating Model Test3</t>
+  </si>
+  <si>
+    <t>Manage Position Trees</t>
+  </si>
+  <si>
+    <t>Setup and Maintenance &gt; Implementation Projects &gt; Workforce Deployment &gt; Define Common Applications Configuration for HCM &gt; Define Enterprise Structures for Human Capital Management &gt; Define Workforce Structures &gt; Define Jobs and Positions &gt; Manage Position Trees</t>
+  </si>
+  <si>
+    <t>Tree Structure</t>
+  </si>
+  <si>
+    <t>Icon Image</t>
+  </si>
+  <si>
+    <t>Base Value</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ACN US POS TREE5</t>
+  </si>
+  <si>
+    <t>ACN_US_POS_TREE5</t>
+  </si>
+  <si>
+    <t>Specify Definition</t>
+  </si>
+  <si>
+    <t>Specify Nodes: Add Tree Node</t>
+  </si>
+  <si>
+    <t>Add again (+): Add Tree Node</t>
+  </si>
+  <si>
+    <t>Tree Name</t>
+  </si>
+  <si>
+    <t>Tree Code</t>
+  </si>
+  <si>
+    <t>*Effective Start Date</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Effective End Date</t>
+  </si>
+  <si>
+    <t>Tree Node</t>
+  </si>
+  <si>
+    <t>*Data Source</t>
+  </si>
+  <si>
+    <t>Add Tree Node</t>
+  </si>
+  <si>
+    <t>ACN POS TEST Tree Version</t>
+  </si>
+  <si>
+    <t>Specific Value</t>
+  </si>
+  <si>
+    <t>Position Tree Data Source</t>
+  </si>
+  <si>
+    <t>ACN POS5</t>
+  </si>
+  <si>
+    <t>ACN POS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Profile Types
+  </t>
+  </si>
+  <si>
+    <t>Setup and Maintenance &gt; Implementation Projects &gt; Workforce Deployment &gt; Define Common Applications Configuration for Human Capital Management &gt; Define Workforce Profiles &gt; Define Talent Profiles &gt; Manage Profile Types</t>
+  </si>
+  <si>
+    <t>Workforce Structures</t>
+  </si>
+  <si>
+    <t>Content Sections</t>
+  </si>
+  <si>
+    <t>*Usage</t>
+  </si>
+  <si>
+    <t>*Workforce Structure</t>
+  </si>
+  <si>
+    <t>AddContentSection</t>
+  </si>
+  <si>
+    <t>Test_Job3</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Profile Type </t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Memberships</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Manage Profile Content Types</t>
+  </si>
+  <si>
+    <t>Setup and Maintenance &gt; Implementation Projects &gt; Workforce Deployment &gt; Define Common Applications Configuration for Human Capital Management &gt; Define Workforce Profiles &gt; Define Talent Profile Content &gt; Manage Profile Content Types</t>
+  </si>
+  <si>
+    <t>Field Properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Name </t>
+  </si>
+  <si>
+    <t>Free Form Type</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>*Label</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Test_Degree4</t>
+  </si>
+  <si>
+    <t>Test Degree4</t>
+  </si>
+  <si>
+    <t>Test Degree</t>
+  </si>
+  <si>
+    <t>ITEM_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Editable</t>
+  </si>
+  <si>
+    <t>ITEM_TEXT_TL_2</t>
+  </si>
+  <si>
+    <t>Month of Education</t>
+  </si>
+  <si>
+    <t>Manage Educational Establishments</t>
+  </si>
+  <si>
+    <t>Setup and Maintenance &gt; Implementation Projects &gt; Workforce Deployment &gt; Define Common Applications Configuration for Human Capital Management &gt; Define Workforce Profiles &gt; Define Talent Profile Content &gt; Manage Educational Establishments</t>
+  </si>
+  <si>
+    <t>*Description</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State Or Province</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>westeros school</t>
+  </si>
+  <si>
+    <t>engg college</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>connecticut</t>
+  </si>
+  <si>
+    <t>NY University</t>
+  </si>
+  <si>
+    <t>Law College</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>texas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode=";;;**"/>
     <numFmt numFmtId="165" formatCode="mm\/dd\/yyyy"/>
+    <numFmt numFmtId="166" formatCode="m\/d\/yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1164,8 +1389,54 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1196,8 +1467,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1352,6 +1653,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1364,7 +1718,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1463,15 +1817,6 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1579,6 +1924,86 @@
     </xf>
     <xf numFmtId="20" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11106,6 +11531,1703 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="148" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="78">
+        <v>32874</v>
+      </c>
+      <c r="E4" s="78">
+        <v>54789</v>
+      </c>
+      <c r="F4" s="78"/>
+      <c r="G4" s="45">
+        <v>1</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="45">
+        <v>2</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="45">
+        <v>3</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" s="46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="45">
+        <v>4</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="45">
+        <v>5</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" s="46">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="F4:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D91"/>
+  <sheetViews>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
+    </row>
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="19" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="19" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="19" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="D33" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>203</v>
+      </c>
+      <c r="C38" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" s="56" t="s">
+        <v>205</v>
+      </c>
+      <c r="C39" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="56" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="57" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="56" t="s">
+        <v>211</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="C45" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D45" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" s="56" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B48" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="D48" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="56" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B50" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="C50" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="D50" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="C51" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="D51" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="D52" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="D53" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="C55" s="57" t="s">
+        <v>238</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="C56" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="D56" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" s="56" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="D57" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="C58" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B59" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="C59" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D59" s="58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="C60" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="D60" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="C61" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="D61" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="C62" s="57" t="s">
+        <v>252</v>
+      </c>
+      <c r="D62" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" s="57" t="s">
+        <v>254</v>
+      </c>
+      <c r="D63" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="C64" s="57" t="s">
+        <v>256</v>
+      </c>
+      <c r="D64" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" s="56" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="D65" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" s="56" t="s">
+        <v>259</v>
+      </c>
+      <c r="C66" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="D66" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="63" t="s">
+        <v>261</v>
+      </c>
+      <c r="C67" s="64" t="s">
+        <v>262</v>
+      </c>
+      <c r="D67" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="63" t="s">
+        <v>263</v>
+      </c>
+      <c r="C68" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="D68" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B69" s="63" t="s">
+        <v>265</v>
+      </c>
+      <c r="C69" s="64" t="s">
+        <v>266</v>
+      </c>
+      <c r="D69" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="C70" s="64" t="s">
+        <v>268</v>
+      </c>
+      <c r="D70" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" s="63" t="s">
+        <v>269</v>
+      </c>
+      <c r="C71" s="64" t="s">
+        <v>270</v>
+      </c>
+      <c r="D71" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="63" t="s">
+        <v>271</v>
+      </c>
+      <c r="C72" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="D72" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" s="63" t="s">
+        <v>273</v>
+      </c>
+      <c r="C73" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="D73" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="63" t="s">
+        <v>275</v>
+      </c>
+      <c r="C74" s="64" t="s">
+        <v>276</v>
+      </c>
+      <c r="D74" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" s="63" t="s">
+        <v>277</v>
+      </c>
+      <c r="C75" s="64" t="s">
+        <v>278</v>
+      </c>
+      <c r="D75" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" s="63" t="s">
+        <v>279</v>
+      </c>
+      <c r="C76" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="D76" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="C77" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="D77" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="66" t="s">
+        <v>283</v>
+      </c>
+      <c r="C78" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="D78" s="68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B79" s="70" t="s">
+        <v>286</v>
+      </c>
+      <c r="C79" s="71" t="s">
+        <v>287</v>
+      </c>
+      <c r="D79" s="72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B80" s="73" t="s">
+        <v>288</v>
+      </c>
+      <c r="C80" s="74" t="s">
+        <v>289</v>
+      </c>
+      <c r="D80" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B81" s="73" t="s">
+        <v>290</v>
+      </c>
+      <c r="C81" s="74" t="s">
+        <v>291</v>
+      </c>
+      <c r="D81" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B82" s="73" t="s">
+        <v>292</v>
+      </c>
+      <c r="C82" s="74" t="s">
+        <v>293</v>
+      </c>
+      <c r="D82" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B83" s="73" t="s">
+        <v>294</v>
+      </c>
+      <c r="C83" s="74" t="s">
+        <v>295</v>
+      </c>
+      <c r="D83" s="72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B84" s="73" t="s">
+        <v>296</v>
+      </c>
+      <c r="C84" s="74" t="s">
+        <v>297</v>
+      </c>
+      <c r="D84" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B85" s="73" t="s">
+        <v>298</v>
+      </c>
+      <c r="C85" s="74" t="s">
+        <v>299</v>
+      </c>
+      <c r="D85" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B86" s="73" t="s">
+        <v>300</v>
+      </c>
+      <c r="C86" s="74" t="s">
+        <v>301</v>
+      </c>
+      <c r="D86" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="B87" s="73" t="s">
+        <v>303</v>
+      </c>
+      <c r="C87" s="74" t="s">
+        <v>304</v>
+      </c>
+      <c r="D87" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="B88" s="73" t="s">
+        <v>305</v>
+      </c>
+      <c r="C88" s="74" t="s">
+        <v>306</v>
+      </c>
+      <c r="D88" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="B89" s="73" t="s">
+        <v>307</v>
+      </c>
+      <c r="C89" s="74" t="s">
+        <v>308</v>
+      </c>
+      <c r="D89" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="B90" s="73" t="s">
+        <v>309</v>
+      </c>
+      <c r="C90" s="74" t="s">
+        <v>310</v>
+      </c>
+      <c r="D90" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="B91" s="73" t="s">
+        <v>311</v>
+      </c>
+      <c r="C91" s="74" t="s">
+        <v>312</v>
+      </c>
+      <c r="D91" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="76" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="77">
+        <v>0.375</v>
+      </c>
+      <c r="E4" s="76">
+        <v>9</v>
+      </c>
+      <c r="F4" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="G4" s="76" t="s">
+        <v>330</v>
+      </c>
+      <c r="H4" s="76" t="s">
+        <v>331</v>
+      </c>
+      <c r="I4" s="76" t="s">
+        <v>332</v>
+      </c>
+      <c r="J4" s="76">
+        <v>1</v>
+      </c>
+      <c r="K4" s="77">
+        <v>0.375</v>
+      </c>
+      <c r="L4" s="76">
+        <v>9</v>
+      </c>
+      <c r="M4" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="N4" s="76">
+        <v>20</v>
+      </c>
+      <c r="O4" s="76">
+        <v>45</v>
+      </c>
+      <c r="P4" s="76" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="77">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="76">
+        <v>9</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" s="76" t="s">
+        <v>330</v>
+      </c>
+      <c r="H5" s="76" t="s">
+        <v>331</v>
+      </c>
+      <c r="I5" s="76" t="s">
+        <v>332</v>
+      </c>
+      <c r="J5" s="76">
+        <v>1</v>
+      </c>
+      <c r="K5" s="77">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L5" s="76">
+        <v>9</v>
+      </c>
+      <c r="M5" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="N5" s="76">
+        <v>15</v>
+      </c>
+      <c r="O5" s="76">
+        <v>30</v>
+      </c>
+      <c r="P5" s="76" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
@@ -11315,13 +13437,13 @@
       <c r="A4" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="78" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="28">
@@ -11347,9 +13469,9 @@
       <c r="A5" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="28">
         <v>20</v>
       </c>
@@ -11373,9 +13495,9 @@
       <c r="A6" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="28">
         <v>30</v>
       </c>
@@ -11537,7 +13659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -11820,227 +13942,187 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="148" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+    <row r="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="C3" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
+        <v>345</v>
+      </c>
+      <c r="B4" s="81" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81" t="s">
+        <v>346</v>
+      </c>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+    </row>
+    <row r="5" spans="1:15" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="82" t="s">
+        <v>347</v>
+      </c>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="82" t="s">
+        <v>348</v>
+      </c>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83" t="s">
+        <v>349</v>
+      </c>
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="84"/>
+    </row>
+    <row r="7" spans="1:15" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>351</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="D7" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="F7" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="46" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>337</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>338</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="41">
-        <v>32874</v>
-      </c>
-      <c r="E4" s="41">
-        <v>54789</v>
-      </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="48">
-        <v>1</v>
-      </c>
-      <c r="H4" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="I4" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="K4" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>337</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="48">
-        <v>2</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="K5" s="49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
-        <v>337</v>
-      </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="48">
-        <v>3</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="J6" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="K6" s="49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
-        <v>337</v>
-      </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="48">
-        <v>4</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="K7" s="49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
-        <v>337</v>
-      </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="48">
-        <v>5</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="J8" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="K8" s="49">
-        <v>5</v>
+      <c r="G7" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="81" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" s="81" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" s="85">
+        <v>18629</v>
+      </c>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81" t="s">
+        <v>358</v>
+      </c>
+      <c r="G8" s="86">
+        <v>1027428</v>
+      </c>
+      <c r="H8" s="87" t="s">
+        <v>359</v>
+      </c>
+      <c r="I8" s="87" t="s">
+        <v>360</v>
+      </c>
+      <c r="J8" s="81" t="s">
+        <v>361</v>
+      </c>
+      <c r="K8" s="87" t="s">
+        <v>359</v>
+      </c>
+      <c r="L8" s="87" t="s">
+        <v>360</v>
+      </c>
+      <c r="M8" s="81" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="F4:F8"/>
+  <mergeCells count="3">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12048,1279 +14130,134 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52"/>
-    </row>
-    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-    </row>
-    <row r="3" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="54" t="s">
+    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="88" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="89" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="91" t="s">
+        <v>365</v>
+      </c>
+      <c r="H2" s="92" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="53" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="D8" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" s="59" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>158</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="C17" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="60" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B19" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="C21" s="60" t="s">
-        <v>169</v>
-      </c>
-      <c r="D21" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B22" s="59" t="s">
-        <v>170</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="59" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="60" t="s">
-        <v>175</v>
-      </c>
-      <c r="D24" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="60" t="s">
-        <v>177</v>
-      </c>
-      <c r="D25" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>178</v>
-      </c>
-      <c r="C26" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="D26" s="64" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B27" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>182</v>
-      </c>
-      <c r="D27" s="58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B28" s="59" t="s">
-        <v>183</v>
-      </c>
-      <c r="C28" s="60" t="s">
-        <v>184</v>
-      </c>
-      <c r="D28" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="19" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B29" s="59" t="s">
-        <v>185</v>
-      </c>
-      <c r="C29" s="60" t="s">
-        <v>186</v>
-      </c>
-      <c r="D29" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B30" s="59" t="s">
-        <v>187</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>188</v>
-      </c>
-      <c r="D30" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="C31" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="D31" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="19" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B32" s="59" t="s">
-        <v>191</v>
-      </c>
-      <c r="C32" s="60" t="s">
-        <v>192</v>
-      </c>
-      <c r="D32" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="19" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B33" s="59" t="s">
-        <v>193</v>
-      </c>
-      <c r="C33" s="60" t="s">
-        <v>194</v>
-      </c>
-      <c r="D33" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B34" s="59" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="D34" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="19" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B35" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="C35" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="D35" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B36" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="C36" s="60" t="s">
-        <v>200</v>
-      </c>
-      <c r="D36" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B37" s="59" t="s">
-        <v>201</v>
-      </c>
-      <c r="C37" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="D37" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B38" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="C38" s="60" t="s">
-        <v>204</v>
-      </c>
-      <c r="D38" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B39" s="59" t="s">
-        <v>205</v>
-      </c>
-      <c r="C39" s="60" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B40" s="59" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="D40" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="59" t="s">
-        <v>209</v>
-      </c>
-      <c r="C41" s="60" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B42" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="C42" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="D42" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B43" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="C43" s="60" t="s">
-        <v>214</v>
-      </c>
-      <c r="D43" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B44" s="59" t="s">
-        <v>215</v>
-      </c>
-      <c r="C44" s="60" t="s">
-        <v>216</v>
-      </c>
-      <c r="D44" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B45" s="59" t="s">
-        <v>217</v>
-      </c>
-      <c r="C45" s="60" t="s">
-        <v>218</v>
-      </c>
-      <c r="D45" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B46" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="C46" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="D46" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B47" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="C47" s="60" t="s">
-        <v>222</v>
-      </c>
-      <c r="D47" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B48" s="59" t="s">
-        <v>223</v>
-      </c>
-      <c r="C48" s="60" t="s">
-        <v>224</v>
-      </c>
-      <c r="D48" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B49" s="59" t="s">
-        <v>225</v>
-      </c>
-      <c r="C49" s="60" t="s">
-        <v>226</v>
-      </c>
-      <c r="D49" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B50" s="59" t="s">
-        <v>227</v>
-      </c>
-      <c r="C50" s="60" t="s">
-        <v>228</v>
-      </c>
-      <c r="D50" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B51" s="59" t="s">
-        <v>229</v>
-      </c>
-      <c r="C51" s="60" t="s">
-        <v>230</v>
-      </c>
-      <c r="D51" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B52" s="59" t="s">
-        <v>231</v>
-      </c>
-      <c r="C52" s="60" t="s">
-        <v>232</v>
-      </c>
-      <c r="D52" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B53" s="59" t="s">
-        <v>233</v>
-      </c>
-      <c r="C53" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="D53" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B54" s="59" t="s">
-        <v>235</v>
-      </c>
-      <c r="C54" s="60" t="s">
-        <v>236</v>
-      </c>
-      <c r="D54" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B55" s="59" t="s">
-        <v>237</v>
-      </c>
-      <c r="C55" s="60" t="s">
-        <v>238</v>
-      </c>
-      <c r="D55" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B56" s="59" t="s">
-        <v>239</v>
-      </c>
-      <c r="C56" s="60" t="s">
-        <v>240</v>
-      </c>
-      <c r="D56" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B57" s="59" t="s">
-        <v>241</v>
-      </c>
-      <c r="C57" s="60" t="s">
-        <v>242</v>
-      </c>
-      <c r="D57" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B58" s="59" t="s">
-        <v>243</v>
-      </c>
-      <c r="C58" s="60" t="s">
-        <v>244</v>
-      </c>
-      <c r="D58" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B59" s="59" t="s">
-        <v>245</v>
-      </c>
-      <c r="C59" s="60" t="s">
-        <v>246</v>
-      </c>
-      <c r="D59" s="61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B60" s="59" t="s">
-        <v>247</v>
-      </c>
-      <c r="C60" s="60" t="s">
-        <v>248</v>
-      </c>
-      <c r="D60" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B61" s="59" t="s">
-        <v>249</v>
-      </c>
-      <c r="C61" s="60" t="s">
-        <v>250</v>
-      </c>
-      <c r="D61" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" s="19" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B62" s="59" t="s">
-        <v>251</v>
-      </c>
-      <c r="C62" s="60" t="s">
-        <v>252</v>
-      </c>
-      <c r="D62" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B63" s="59" t="s">
-        <v>253</v>
-      </c>
-      <c r="C63" s="60" t="s">
-        <v>254</v>
-      </c>
-      <c r="D63" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B64" s="59" t="s">
-        <v>255</v>
-      </c>
-      <c r="C64" s="60" t="s">
-        <v>256</v>
-      </c>
-      <c r="D64" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B65" s="59" t="s">
-        <v>257</v>
-      </c>
-      <c r="C65" s="60" t="s">
-        <v>258</v>
-      </c>
-      <c r="D65" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="B66" s="59" t="s">
-        <v>259</v>
-      </c>
-      <c r="C66" s="60" t="s">
-        <v>260</v>
-      </c>
-      <c r="D66" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B67" s="66" t="s">
-        <v>261</v>
-      </c>
-      <c r="C67" s="67" t="s">
-        <v>262</v>
-      </c>
-      <c r="D67" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B68" s="66" t="s">
-        <v>263</v>
-      </c>
-      <c r="C68" s="67" t="s">
-        <v>264</v>
-      </c>
-      <c r="D68" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B69" s="66" t="s">
-        <v>265</v>
-      </c>
-      <c r="C69" s="67" t="s">
-        <v>266</v>
-      </c>
-      <c r="D69" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B70" s="66" t="s">
-        <v>267</v>
-      </c>
-      <c r="C70" s="67" t="s">
-        <v>268</v>
-      </c>
-      <c r="D70" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B71" s="66" t="s">
-        <v>269</v>
-      </c>
-      <c r="C71" s="67" t="s">
-        <v>270</v>
-      </c>
-      <c r="D71" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B72" s="66" t="s">
-        <v>271</v>
-      </c>
-      <c r="C72" s="67" t="s">
-        <v>272</v>
-      </c>
-      <c r="D72" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="66" t="s">
-        <v>273</v>
-      </c>
-      <c r="C73" s="67" t="s">
-        <v>274</v>
-      </c>
-      <c r="D73" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B74" s="66" t="s">
-        <v>275</v>
-      </c>
-      <c r="C74" s="67" t="s">
-        <v>276</v>
-      </c>
-      <c r="D74" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B75" s="66" t="s">
-        <v>277</v>
-      </c>
-      <c r="C75" s="67" t="s">
-        <v>278</v>
-      </c>
-      <c r="D75" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B76" s="66" t="s">
-        <v>279</v>
-      </c>
-      <c r="C76" s="67" t="s">
-        <v>280</v>
-      </c>
-      <c r="D76" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B77" s="66" t="s">
-        <v>281</v>
-      </c>
-      <c r="C77" s="67" t="s">
-        <v>282</v>
-      </c>
-      <c r="D77" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="B78" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="C78" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="D78" s="71" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B79" s="73" t="s">
-        <v>286</v>
-      </c>
-      <c r="C79" s="74" t="s">
-        <v>287</v>
-      </c>
-      <c r="D79" s="75" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B80" s="76" t="s">
-        <v>288</v>
-      </c>
-      <c r="C80" s="77" t="s">
-        <v>289</v>
-      </c>
-      <c r="D80" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B81" s="76" t="s">
-        <v>290</v>
-      </c>
-      <c r="C81" s="77" t="s">
-        <v>291</v>
-      </c>
-      <c r="D81" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B82" s="76" t="s">
-        <v>292</v>
-      </c>
-      <c r="C82" s="77" t="s">
-        <v>293</v>
-      </c>
-      <c r="D82" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B83" s="76" t="s">
-        <v>294</v>
-      </c>
-      <c r="C83" s="77" t="s">
-        <v>295</v>
-      </c>
-      <c r="D83" s="75" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B84" s="76" t="s">
-        <v>296</v>
-      </c>
-      <c r="C84" s="77" t="s">
-        <v>297</v>
-      </c>
-      <c r="D84" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B85" s="76" t="s">
-        <v>298</v>
-      </c>
-      <c r="C85" s="77" t="s">
-        <v>299</v>
-      </c>
-      <c r="D85" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B86" s="76" t="s">
-        <v>300</v>
-      </c>
-      <c r="C86" s="77" t="s">
-        <v>301</v>
-      </c>
-      <c r="D86" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B87" s="76" t="s">
-        <v>303</v>
-      </c>
-      <c r="C87" s="77" t="s">
-        <v>304</v>
-      </c>
-      <c r="D87" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B88" s="76" t="s">
-        <v>305</v>
-      </c>
-      <c r="C88" s="77" t="s">
-        <v>306</v>
-      </c>
-      <c r="D88" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" s="19" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B89" s="76" t="s">
-        <v>307</v>
-      </c>
-      <c r="C89" s="77" t="s">
-        <v>308</v>
-      </c>
-      <c r="D89" s="68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" s="19" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B90" s="76" t="s">
-        <v>309</v>
-      </c>
-      <c r="C90" s="77" t="s">
-        <v>310</v>
-      </c>
-      <c r="D90" s="68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B91" s="76" t="s">
-        <v>311</v>
-      </c>
-      <c r="C91" s="77" t="s">
-        <v>312</v>
-      </c>
-      <c r="D91" s="68" t="s">
-        <v>7</v>
+      <c r="F3" s="94" t="s">
+        <v>367</v>
+      </c>
+      <c r="G3" s="92" t="s">
+        <v>368</v>
+      </c>
+      <c r="H3" s="91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="C4" s="95">
+        <v>18264</v>
+      </c>
+      <c r="D4" s="95">
+        <v>1027428</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="22" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -13330,184 +14267,215 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="B3" s="16" t="s">
+    <row r="1" spans="1:10" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="19" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="97" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="98" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99" t="s">
+        <v>381</v>
+      </c>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="101"/>
+    </row>
+    <row r="3" spans="1:10" s="103" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="102" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>316</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>318</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>324</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="B4" s="79" t="s">
-        <v>327</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>328</v>
-      </c>
-      <c r="D4" s="80">
-        <v>0.375</v>
-      </c>
-      <c r="E4" s="79">
-        <v>9</v>
-      </c>
-      <c r="F4" s="79" t="s">
-        <v>329</v>
-      </c>
-      <c r="G4" s="79" t="s">
-        <v>330</v>
-      </c>
-      <c r="H4" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I4" s="79" t="s">
-        <v>332</v>
-      </c>
-      <c r="J4" s="79">
-        <v>1</v>
-      </c>
-      <c r="K4" s="80">
-        <v>0.375</v>
-      </c>
-      <c r="L4" s="79">
-        <v>9</v>
-      </c>
-      <c r="M4" s="79" t="s">
-        <v>329</v>
-      </c>
-      <c r="N4" s="79">
-        <v>20</v>
-      </c>
-      <c r="O4" s="79">
-        <v>45</v>
-      </c>
-      <c r="P4" s="79" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
-        <v>336</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>327</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>334</v>
-      </c>
-      <c r="D5" s="80">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E5" s="79">
-        <v>9</v>
-      </c>
-      <c r="F5" s="79" t="s">
-        <v>329</v>
-      </c>
-      <c r="G5" s="79" t="s">
-        <v>330</v>
-      </c>
-      <c r="H5" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I5" s="79" t="s">
-        <v>332</v>
-      </c>
-      <c r="J5" s="79">
-        <v>1</v>
-      </c>
-      <c r="K5" s="80">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L5" s="79">
-        <v>9</v>
-      </c>
-      <c r="M5" s="79" t="s">
-        <v>329</v>
-      </c>
-      <c r="N5" s="79">
-        <v>15</v>
-      </c>
-      <c r="O5" s="79">
-        <v>30</v>
-      </c>
-      <c r="P5" s="79" t="s">
-        <v>333</v>
+      <c r="D3" s="102" t="s">
+        <v>383</v>
+      </c>
+      <c r="E3" s="102" t="s">
+        <v>384</v>
+      </c>
+      <c r="F3" s="102" t="s">
+        <v>385</v>
+      </c>
+      <c r="G3" s="102" t="s">
+        <v>386</v>
+      </c>
+      <c r="H3" s="102" t="s">
+        <v>387</v>
+      </c>
+      <c r="I3" s="102" t="s">
+        <v>388</v>
+      </c>
+      <c r="J3" s="102" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="103" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="104" t="s">
+        <v>390</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>392</v>
+      </c>
+      <c r="D4" s="104" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="105" t="s">
+        <v>393</v>
+      </c>
+      <c r="F4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="105" t="s">
+        <v>394</v>
+      </c>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:10" s="103" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="104" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="105" t="s">
+        <v>395</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>396</v>
+      </c>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="105" t="s">
+        <v>394</v>
+      </c>
+      <c r="J5" s="105"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>112233</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
+        <v>223344</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>